<commit_message>
Added missing comments in function
</commit_message>
<xml_diff>
--- a/DemoSolution/FileReadingDemo/TestBook.xlsx
+++ b/DemoSolution/FileReadingDemo/TestBook.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\users\daniel.flores\source\repos\DemoSolution\FileReadingDemo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniel.flores\Documents\Copia del repositorio remoto\DemoRepository\DemoSolution\FileReadingDemo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8516B7FB-54DB-41AC-A3D8-0C2402430FC6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7583A0D6-B89D-4A26-90A4-E30C65265140}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{47E68E66-B82F-48F0-8CE9-59329520423C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="74">
   <si>
     <t>Test values</t>
   </si>
@@ -33,205 +33,220 @@
     <t>Find me</t>
   </si>
   <si>
-    <t>242</t>
-  </si>
-  <si>
-    <t>129</t>
-  </si>
-  <si>
-    <t>470</t>
-  </si>
-  <si>
-    <t>613</t>
-  </si>
-  <si>
-    <t>572</t>
-  </si>
-  <si>
-    <t>971</t>
-  </si>
-  <si>
-    <t>598</t>
-  </si>
-  <si>
-    <t>67</t>
-  </si>
-  <si>
     <t>353</t>
   </si>
   <si>
-    <t>63</t>
-  </si>
-  <si>
-    <t>886</t>
-  </si>
-  <si>
-    <t>101</t>
-  </si>
-  <si>
-    <t>753</t>
-  </si>
-  <si>
-    <t>237</t>
-  </si>
-  <si>
-    <t>656</t>
-  </si>
-  <si>
-    <t>636</t>
-  </si>
-  <si>
-    <t>839</t>
-  </si>
-  <si>
-    <t>787</t>
-  </si>
-  <si>
-    <t>737</t>
-  </si>
-  <si>
-    <t>437</t>
-  </si>
-  <si>
-    <t>121</t>
-  </si>
-  <si>
-    <t>850</t>
-  </si>
-  <si>
-    <t>814</t>
-  </si>
-  <si>
-    <t>220</t>
-  </si>
-  <si>
-    <t>912</t>
-  </si>
-  <si>
     <t>512</t>
   </si>
   <si>
-    <t>309</t>
-  </si>
-  <si>
-    <t>610</t>
-  </si>
-  <si>
-    <t>703</t>
-  </si>
-  <si>
-    <t>882</t>
-  </si>
-  <si>
-    <t>540</t>
-  </si>
-  <si>
-    <t>197</t>
-  </si>
-  <si>
-    <t>60</t>
-  </si>
-  <si>
-    <t>175</t>
-  </si>
-  <si>
-    <t>371</t>
-  </si>
-  <si>
-    <t>935</t>
-  </si>
-  <si>
-    <t>539</t>
-  </si>
-  <si>
-    <t>51</t>
-  </si>
-  <si>
-    <t>97</t>
-  </si>
-  <si>
-    <t>164</t>
-  </si>
-  <si>
-    <t>548</t>
-  </si>
-  <si>
-    <t>893</t>
-  </si>
-  <si>
-    <t>571</t>
-  </si>
-  <si>
     <t>85</t>
   </si>
   <si>
-    <t>440</t>
-  </si>
-  <si>
     <t>166</t>
   </si>
   <si>
-    <t>243</t>
-  </si>
-  <si>
-    <t>623</t>
-  </si>
-  <si>
-    <t>930</t>
-  </si>
-  <si>
-    <t>778</t>
-  </si>
-  <si>
-    <t>620</t>
-  </si>
-  <si>
-    <t>427</t>
-  </si>
-  <si>
-    <t>909</t>
-  </si>
-  <si>
-    <t>701</t>
-  </si>
-  <si>
-    <t>663</t>
-  </si>
-  <si>
-    <t>987</t>
-  </si>
-  <si>
-    <t>364</t>
-  </si>
-  <si>
-    <t>523</t>
-  </si>
-  <si>
-    <t>690</t>
-  </si>
-  <si>
-    <t>41</t>
-  </si>
-  <si>
-    <t>578</t>
-  </si>
-  <si>
-    <t>866</t>
-  </si>
-  <si>
-    <t>720</t>
-  </si>
-  <si>
-    <t>597</t>
-  </si>
-  <si>
-    <t>641</t>
-  </si>
-  <si>
     <t>273</t>
   </si>
   <si>
-    <t>465</t>
+    <t>211</t>
+  </si>
+  <si>
+    <t>746</t>
+  </si>
+  <si>
+    <t>157</t>
+  </si>
+  <si>
+    <t>758</t>
+  </si>
+  <si>
+    <t>932</t>
+  </si>
+  <si>
+    <t>877</t>
+  </si>
+  <si>
+    <t>210</t>
+  </si>
+  <si>
+    <t>232</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>606</t>
+  </si>
+  <si>
+    <t>223</t>
+  </si>
+  <si>
+    <t>805</t>
+  </si>
+  <si>
+    <t>493</t>
+  </si>
+  <si>
+    <t>646</t>
+  </si>
+  <si>
+    <t>356</t>
+  </si>
+  <si>
+    <t>387</t>
+  </si>
+  <si>
+    <t>276</t>
+  </si>
+  <si>
+    <t>317</t>
+  </si>
+  <si>
+    <t>552</t>
+  </si>
+  <si>
+    <t>608</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>235</t>
+  </si>
+  <si>
+    <t>161</t>
+  </si>
+  <si>
+    <t>798</t>
+  </si>
+  <si>
+    <t>524</t>
+  </si>
+  <si>
+    <t>772</t>
+  </si>
+  <si>
+    <t>961</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>405</t>
+  </si>
+  <si>
+    <t>829</t>
+  </si>
+  <si>
+    <t>93</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>887</t>
+  </si>
+  <si>
+    <t>475</t>
+  </si>
+  <si>
+    <t>149</t>
+  </si>
+  <si>
+    <t>436</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>664</t>
+  </si>
+  <si>
+    <t>130</t>
+  </si>
+  <si>
+    <t>926</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>760</t>
+  </si>
+  <si>
+    <t>634</t>
+  </si>
+  <si>
+    <t>659</t>
+  </si>
+  <si>
+    <t>647</t>
+  </si>
+  <si>
+    <t>518</t>
+  </si>
+  <si>
+    <t>217</t>
+  </si>
+  <si>
+    <t>655</t>
+  </si>
+  <si>
+    <t>432</t>
+  </si>
+  <si>
+    <t>322</t>
+  </si>
+  <si>
+    <t>244</t>
+  </si>
+  <si>
+    <t>996</t>
+  </si>
+  <si>
+    <t>960</t>
+  </si>
+  <si>
+    <t>409</t>
+  </si>
+  <si>
+    <t>106</t>
+  </si>
+  <si>
+    <t>249</t>
+  </si>
+  <si>
+    <t>239</t>
+  </si>
+  <si>
+    <t>826</t>
+  </si>
+  <si>
+    <t>189</t>
+  </si>
+  <si>
+    <t>514</t>
+  </si>
+  <si>
+    <t>167</t>
+  </si>
+  <si>
+    <t>917</t>
+  </si>
+  <si>
+    <t>171</t>
+  </si>
+  <si>
+    <t>208</t>
+  </si>
+  <si>
+    <t>950</t>
+  </si>
+  <si>
+    <t>261</t>
+  </si>
+  <si>
+    <t>478</t>
   </si>
 </sst>
 </file>
@@ -602,91 +617,91 @@
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <f ca="1">RAND()*1000</f>
-        <v>736.74952639661467</v>
+        <v>214.15514234629097</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ref="A3:A20" ca="1" si="0">RAND()*1000</f>
-        <v>500.81421951413449</v>
+        <v>90.76156503417954</v>
       </c>
       <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ca="1" si="0"/>
-        <v>403.1653136522616</v>
+        <v>330.60317606788169</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ca="1" si="0"/>
-        <v>627.04713409132876</v>
+        <v>482.48978807777053</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" ca="1" si="0"/>
-        <v>401.32101649592732</v>
+        <v>952.58090641442766</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -694,88 +709,88 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" ca="1" si="0"/>
-        <v>438.06502941391136</v>
+        <v>40.340657097058582</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" ca="1" si="0"/>
-        <v>313.8756555539378</v>
+        <v>151.61728940007947</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E9" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" ca="1" si="0"/>
-        <v>600.47985751183126</v>
+        <v>236.31933083345459</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="E10" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" ca="1" si="0"/>
-        <v>280.96325114052178</v>
+        <v>935.06493958027102</v>
       </c>
       <c r="B11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" t="s">
         <v>38</v>
-      </c>
-      <c r="C11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -783,160 +798,160 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="D12" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E12" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" ca="1" si="0"/>
-        <v>165.21376605705797</v>
+        <v>232.72875888617605</v>
       </c>
       <c r="B13" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D13" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E13" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" ca="1" si="0"/>
-        <v>675.42001528179173</v>
+        <v>304.15478846305786</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D14" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" ca="1" si="0"/>
-        <v>289.34653065197648</v>
+        <v>322.62852033436127</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C15" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D15" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E15" t="s">
-        <v>52</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" ca="1" si="0"/>
-        <v>700.82754517084777</v>
+        <v>301.80939546576036</v>
       </c>
       <c r="B16" t="s">
-        <v>53</v>
+        <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D16" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="E16" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" ca="1" si="0"/>
-        <v>113.46900491710976</v>
+        <v>72.69948006566851</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C17" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="D17" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="E17" t="s">
-        <v>4</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" ca="1" si="0"/>
-        <v>275.02676211038255</v>
+        <v>159.06203599549062</v>
       </c>
       <c r="B18" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="C18" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="D18" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="E18" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" ca="1" si="0"/>
-        <v>901.23391405187192</v>
+        <v>22.027861261727733</v>
       </c>
       <c r="B19" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C19" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D19" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="E19" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" ca="1" si="0"/>
-        <v>356.67487715506616</v>
+        <v>891.8949850962897</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="C20" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D20" t="s">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="E20" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>